<commit_message>
Updated stats and classes implementation
</commit_message>
<xml_diff>
--- a/FEArena/classes.xlsx
+++ b/FEArena/classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\HEROBOOK\Users\k_hom\Documents\Seneca\Repos\Fire Emblem Arena\FEArena\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{052B57D7-9686-471A-8EE0-293646E36EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD288D61-E534-49AA-BAC5-7BD0965ED3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2535" windowWidth="24240" windowHeight="13140" xr2:uid="{85E96280-5E1B-4E00-BBB1-6BDE1EDD9B4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85E96280-5E1B-4E00-BBB1-6BDE1EDD9B4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
   <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -646,7 +646,7 @@
       </c>
       <c r="L2" s="1">
         <f>SUM(D2:K2)</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M2">
         <v>75</v>
@@ -658,26 +658,26 @@
         <v>40</v>
       </c>
       <c r="P2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="Q2">
         <v>30</v>
       </c>
       <c r="R2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S2">
         <v>15</v>
       </c>
       <c r="T2" s="1">
         <f>SUM(M2:S2)</f>
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="U2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -709,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -734,7 +734,7 @@
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L15" si="0">SUM(D3:K3)</f>
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="M3">
         <v>80</v>
@@ -752,14 +752,14 @@
         <v>25</v>
       </c>
       <c r="R3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="S3">
         <v>20</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" ref="T3:T15" si="1">SUM(M3:S3)</f>
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -800,13 +800,13 @@
         <v>18</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4">
         <v>80</v>
@@ -831,23 +831,23 @@
         <v>40</v>
       </c>
       <c r="O4">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="P4">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R4">
         <v>20</v>
       </c>
       <c r="S4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="T4" s="1">
         <f t="shared" si="1"/>
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="U4">
         <v>31</v>
@@ -900,23 +900,23 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>8</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M5">
         <v>70</v>
       </c>
       <c r="N5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O5">
         <v>40</v>
@@ -925,7 +925,7 @@
         <v>40</v>
       </c>
       <c r="Q5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R5">
         <v>15</v>
@@ -979,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>9</v>
@@ -991,39 +991,39 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <v>6</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M6">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="N6">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O6">
         <v>45</v>
       </c>
       <c r="P6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="Q6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="R6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S6">
         <v>20</v>
       </c>
       <c r="T6" s="1">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="U6">
         <v>31</v>
@@ -1064,13 +1064,13 @@
         <v>18</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1079,14 +1079,14 @@
         <v>3</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>7</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="M7">
         <v>70</v>
@@ -1095,7 +1095,7 @@
         <v>35</v>
       </c>
       <c r="O7">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="P7">
         <v>35</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="T7" s="1">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -1152,10 +1152,10 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -1167,14 +1167,14 @@
         <v>2</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8">
         <v>7</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="M8">
         <v>75</v>
@@ -1195,11 +1195,11 @@
         <v>10</v>
       </c>
       <c r="S8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="T8" s="1">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1240,19 +1240,19 @@
         <v>16</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
       </c>
       <c r="J9">
         <v>3</v>
@@ -1262,32 +1262,32 @@
       </c>
       <c r="L9" s="1">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="M9">
         <v>55</v>
       </c>
       <c r="N9">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O9">
         <v>40</v>
       </c>
       <c r="P9">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="Q9">
         <v>20</v>
       </c>
       <c r="R9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S9">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="T9" s="1">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1325,16 +1325,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1350,32 +1350,32 @@
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="M10">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="N10">
+        <v>40</v>
+      </c>
+      <c r="O10">
         <v>30</v>
       </c>
-      <c r="O10">
-        <v>35</v>
-      </c>
       <c r="P10">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q10">
         <v>45</v>
       </c>
       <c r="R10">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S10">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="T10" s="1">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -1413,13 +1413,13 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -1428,26 +1428,26 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11">
         <v>7</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="M11">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="N11">
         <v>50</v>
       </c>
       <c r="O11">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="P11">
         <v>30</v>
@@ -1456,14 +1456,14 @@
         <v>20</v>
       </c>
       <c r="R11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="S11">
         <v>30</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="1"/>
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -1501,16 +1501,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1519,23 +1519,23 @@
         <v>3</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K12">
         <v>5</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="M12">
         <v>65</v>
       </c>
       <c r="N12">
+        <v>30</v>
+      </c>
+      <c r="O12">
         <v>35</v>
-      </c>
-      <c r="O12">
-        <v>40</v>
       </c>
       <c r="P12">
         <v>40</v>
@@ -1544,14 +1544,14 @@
         <v>35</v>
       </c>
       <c r="R12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="S12">
         <v>35</v>
       </c>
       <c r="T12" s="1">
         <f t="shared" si="1"/>
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>7</v>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1614,16 +1614,16 @@
       </c>
       <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>65</v>
       </c>
       <c r="N13">
+        <v>45</v>
+      </c>
+      <c r="O13">
         <v>35</v>
-      </c>
-      <c r="O13">
-        <v>30</v>
       </c>
       <c r="P13">
         <v>30</v>
@@ -1632,14 +1632,14 @@
         <v>25</v>
       </c>
       <c r="R13">
+        <v>35</v>
+      </c>
+      <c r="S13">
         <v>15</v>
-      </c>
-      <c r="S13">
-        <v>17</v>
       </c>
       <c r="T13" s="1">
         <f t="shared" si="1"/>
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -1680,19 +1680,19 @@
         <v>20</v>
       </c>
       <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
         <v>5</v>
       </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>4</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="L14" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="M14">
         <v>85</v>
@@ -1720,10 +1720,10 @@
         <v>15</v>
       </c>
       <c r="R14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="T14" s="1">
         <f t="shared" si="1"/>
@@ -1768,13 +1768,13 @@
         <v>20</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1790,19 +1790,19 @@
       </c>
       <c r="L15" s="1">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="M15">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="N15">
         <v>50</v>
       </c>
       <c r="O15">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P15">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="Q15">
         <v>15</v>
@@ -1811,11 +1811,11 @@
         <v>10</v>
       </c>
       <c r="S15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="T15" s="1">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="U15">
         <v>0</v>

</xml_diff>